<commit_message>
updated readme & added main
</commit_message>
<xml_diff>
--- a/Analysis/model_metrics_comparison.xlsx
+++ b/Analysis/model_metrics_comparison.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -522,118 +522,118 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Linear Regression</t>
+          <t>Derived RF</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1289.095 ± 73.486</t>
+          <t>221.298 ± 16.550</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.481 ± 0.015</t>
+          <t>0.911 ± 0.004</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>15181.886 ± 630.461</t>
+          <t>1201.131 ± 173.401</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.335 ± 0.020</t>
+          <t>0.947 ± 0.008</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>19870.765 ± 654.413</t>
+          <t>1829.821 ± 129.676</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>0.393 ± 0.020</t>
+          <t>0.944 ± 0.003</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Multi-Output RF</t>
+          <t>Derived XGBoost</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1084.083 ± 91.274</t>
+          <t>178.397 ± 6.878</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.934 ± 0.002</t>
+          <t>0.928 ± 0.003</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1084.083 ± 91.274</t>
+          <t>984.704 ± 103.751</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.934 ± 0.002</t>
+          <t>0.957 ± 0.005</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>1084.083 ± 91.274</t>
+          <t>1378.546 ± 96.719</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0.934 ± 0.002</t>
+          <t>0.958 ± 0.003</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Multi-Output XGBoost</t>
+          <t>Linear Regression</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>847.215 ± 66.448</t>
+          <t>1289.095 ± 73.486</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.948 ± 0.002</t>
+          <t>0.481 ± 0.015</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>847.215 ± 66.448</t>
+          <t>15181.886 ± 630.461</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.948 ± 0.002</t>
+          <t>0.335 ± 0.020</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>847.215 ± 66.448</t>
+          <t>19870.765 ± 654.413</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0.948 ± 0.002</t>
+          <t>0.393 ± 0.020</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Random Forest</t>
+          <t>Multi-Output RF</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -670,35 +670,109 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
+          <t>Multi-Output XGBoost</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>178.397 ± 6.878</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0.928 ± 0.003</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>984.704 ± 103.751</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0.957 ± 0.005</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>1378.546 ± 96.719</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0.958 ± 0.003</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Random Forest</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>221.298 ± 16.550</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0.911 ± 0.004</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>1201.131 ± 173.401</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>0.947 ± 0.008</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>1829.821 ± 129.676</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>0.944 ± 0.003</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
           <t>XGBoost</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>178.397 ± 6.878</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>0.928 ± 0.003</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>984.704 ± 103.751</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>0.957 ± 0.005</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>1378.546 ± 96.719</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>0.958 ± 0.003</t>
         </is>

</xml_diff>